<commit_message>
Added column to inhibitor files
Now extracting smiles string in a new column.
</commit_message>
<xml_diff>
--- a/inhibitors/CORDATA/avionics_dataset.xlsx
+++ b/inhibitors/CORDATA/avionics_dataset.xlsx
@@ -1,31 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Projekte\Weiterbildung\Quantum_Computing\2024_airbus_challenge\CORDATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Projekte\Weiterbildung\Quantum_Computing\2024_airbus_challenge\git\2024_inhibitQ-main\inhibitors\CORDATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DCC429-3FF6-480D-9A35-6BE01E5D9644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A245611-9EA7-4DA6-80CB-907BCC3DCBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List avionics" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="101">
   <si>
     <t>pH</t>
   </si>
@@ -325,6 +358,9 @@
   </si>
   <si>
     <t>98.3</t>
+  </si>
+  <si>
+    <t>Smiles</t>
   </si>
 </sst>
 </file>
@@ -425,7 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -496,6 +532,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -777,18 +815,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CB5768-AAC2-4F55-A1CE-846DCE7E2E85}">
-  <dimension ref="A1:H126"/>
+  <sheetPr codeName="Tabelle1"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I2" sqref="I2:I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="9" max="9" width="28.109375" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -813,8 +853,11 @@
       <c r="H1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -839,8 +882,12 @@
       <c r="H2" s="23">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2" s="25" t="str" cm="1">
+        <f t="array" ref="I2">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B2), SEARCH("model=",GetURL(B2))+5+1, (SEARCH("/#",GetURL(B2)))-(SEARCH("model=",GetURL(B2))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>OC(=O)CS</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -865,8 +912,12 @@
       <c r="H3" s="7">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="25" t="str" cm="1">
+        <f t="array" ref="I3">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B3), SEARCH("model=",GetURL(B3))+5+1, (SEARCH("/#",GetURL(B3)))-(SEARCH("model=",GetURL(B3))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>Sc1nc2c([nH]1)cccc2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -891,8 +942,12 @@
       <c r="H4" s="10">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="25" t="str" cm="1">
+        <f t="array" ref="I4">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B4), SEARCH("model=",GetURL(B4))+5+1, (SEARCH("/#",GetURL(B4)))-(SEARCH("model=",GetURL(B4))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>S=c1sc2c([nH]1)cccc2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -917,8 +972,12 @@
       <c r="H5" s="7">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="25" t="str" cm="1">
+        <f t="array" ref="I5">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B5), SEARCH("model=",GetURL(B5))+5+1, (SEARCH("/#",GetURL(B5)))-(SEARCH("model=",GetURL(B5))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>S=c1sc2c([nH]1)cccc2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -943,8 +1002,12 @@
       <c r="H6" s="10">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="25" t="str" cm="1">
+        <f t="array" ref="I6">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B6), SEARCH("model=",GetURL(B6))+5+1, (SEARCH("/#",GetURL(B6)))-(SEARCH("model=",GetURL(B6))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>OC(=O)CCS</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -969,8 +1032,12 @@
       <c r="H7" s="7">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="25" t="str" cm="1">
+        <f t="array" ref="I7">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B7), SEARCH("model=",GetURL(B7))+5+1, (SEARCH("/#",GetURL(B7)))-(SEARCH("model=",GetURL(B7))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>OC(=O)c1ccc(cc1)S</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -995,8 +1062,12 @@
       <c r="H8" s="10">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="25" t="str" cm="1">
+        <f t="array" ref="I8">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B8), SEARCH("model=",GetURL(B8))+5+1, (SEARCH("/#",GetURL(B8)))-(SEARCH("model=",GetURL(B8))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>Nc1ccc2c(c1)sc(=S)[nH]2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1021,8 +1092,12 @@
       <c r="H9" s="7">
         <v>94</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="25" t="str" cm="1">
+        <f t="array" ref="I9">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B9), SEARCH("model=",GetURL(B9))+5+1, (SEARCH("/#",GetURL(B9)))-(SEARCH("model=",GetURL(B9))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>OC(=O)c1ccc(=S)[nH]c1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1047,8 +1122,12 @@
       <c r="H10" s="10">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="25" t="str" cm="1">
+        <f t="array" ref="I10">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B10), SEARCH("model=",GetURL(B10))+5+1, (SEARCH("/#",GetURL(B10)))-(SEARCH("model=",GetURL(B10))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>c1ccc2c(c1)[nH]nn2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1073,8 +1152,12 @@
       <c r="H11" s="7">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="25" t="str" cm="1">
+        <f t="array" ref="I11">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B11), SEARCH("model=",GetURL(B11))+5+1, (SEARCH("/#",GetURL(B11)))-(SEARCH("model=",GetURL(B11))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>c1ccc2c(c1)[nH]nn2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1099,8 +1182,12 @@
       <c r="H12" s="10">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I12" s="25" t="str" cm="1">
+        <f t="array" ref="I12">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B12), SEARCH("model=",GetURL(B12))+5+1, (SEARCH("/#",GetURL(B12)))-(SEARCH("model=",GetURL(B12))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCN(C(=S)S)CC</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1125,8 +1212,12 @@
       <c r="H13" s="7">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I13" s="25" t="str" cm="1">
+        <f t="array" ref="I13">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B13), SEARCH("model=",GetURL(B13))+5+1, (SEARCH("/#",GetURL(B13)))-(SEARCH("model=",GetURL(B13))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCN(C(=S)S)CC</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -1151,8 +1242,12 @@
       <c r="H14" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="25" t="str" cm="1">
+        <f t="array" ref="I14">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B14), SEARCH("model=",GetURL(B14))+5+1, (SEARCH("/#",GetURL(B14)))-(SEARCH("model=",GetURL(B14))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC(=C(C=C1SSC2=CC(=C(C=C2)[N+](=O)[O-])C(=O)O)C(=O)O)[N+](=O)[O-]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1177,8 +1272,13 @@
       <c r="H15" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="25" t="str" cm="1">
+        <f t="array" ref="I15">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B15), SEARCH("model=",GetURL(B15))+5+1, (SEARCH("/#",GetURL(B15)))-(SEARCH("model=",GetURL(B15))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC(=C(C=C1SSC2=CC(=C(C=C2)[N+](=O)[O-])C(=O)O)C(=O)O)[N+](=O)[O-]</v>
+      </c>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -1203,8 +1303,12 @@
       <c r="H16" s="10">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="25" t="str" cm="1">
+        <f t="array" ref="I16">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B16), SEARCH("model=",GetURL(B16))+5+1, (SEARCH("/#",GetURL(B16)))-(SEARCH("model=",GetURL(B16))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC(=C(C=C1SSC2=CC(=C(C=C2)[N+](=O)[O-])C(=O)O)C(=O)O)[N+](=O)[O-]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1229,8 +1333,12 @@
       <c r="H17" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="25" t="str" cm="1">
+        <f t="array" ref="I17">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B17), SEARCH("model=",GetURL(B17))+5+1, (SEARCH("/#",GetURL(B17)))-(SEARCH("model=",GetURL(B17))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC(=C(C=C1SSC2=CC(=C(C=C2)[N+](=O)[O-])C(=O)O)C(=O)O)[N+](=O)[O-]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -1255,8 +1363,12 @@
       <c r="H18" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="25" t="str" cm="1">
+        <f t="array" ref="I18">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B18), SEARCH("model=",GetURL(B18))+5+1, (SEARCH("/#",GetURL(B18)))-(SEARCH("model=",GetURL(B18))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)[O-].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1281,8 +1393,12 @@
       <c r="H19" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="25" t="str" cm="1">
+        <f t="array" ref="I19">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B19), SEARCH("model=",GetURL(B19))+5+1, (SEARCH("/#",GetURL(B19)))-(SEARCH("model=",GetURL(B19))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)[O-].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -1307,8 +1423,12 @@
       <c r="H20" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="25" t="str" cm="1">
+        <f t="array" ref="I20">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B20), SEARCH("model=",GetURL(B20))+5+1, (SEARCH("/#",GetURL(B20)))-(SEARCH("model=",GetURL(B20))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)[O-].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1333,8 +1453,12 @@
       <c r="H21" s="7">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="25" t="str" cm="1">
+        <f t="array" ref="I21">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B21), SEARCH("model=",GetURL(B21))+5+1, (SEARCH("/#",GetURL(B21)))-(SEARCH("model=",GetURL(B21))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)[O-].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1359,8 +1483,12 @@
       <c r="H22" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="25" t="str" cm="1">
+        <f t="array" ref="I22">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B22), SEARCH("model=",GetURL(B22))+5+1, (SEARCH("/#",GetURL(B22)))-(SEARCH("model=",GetURL(B22))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)[O-].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1385,8 +1513,12 @@
       <c r="H23" s="7">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="25" t="str" cm="1">
+        <f t="array" ref="I23">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B23), SEARCH("model=",GetURL(B23))+5+1, (SEARCH("/#",GetURL(B23)))-(SEARCH("model=",GetURL(B23))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)[O-].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -1411,8 +1543,12 @@
       <c r="H24" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="25" t="str" cm="1">
+        <f t="array" ref="I24">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B24), SEARCH("model=",GetURL(B24))+5+1, (SEARCH("/#",GetURL(B24)))-(SEARCH("model=",GetURL(B24))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)[O-].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1437,8 +1573,12 @@
       <c r="H25" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I25" s="25" t="str" cm="1">
+        <f t="array" ref="I25">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B25), SEARCH("model=",GetURL(B25))+5+1, (SEARCH("/#",GetURL(B25)))-(SEARCH("model=",GetURL(B25))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
         <v>25</v>
       </c>
@@ -1463,8 +1603,12 @@
       <c r="H26" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I26" s="25" t="str" cm="1">
+        <f t="array" ref="I26">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B26), SEARCH("model=",GetURL(B26))+5+1, (SEARCH("/#",GetURL(B26)))-(SEARCH("model=",GetURL(B26))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1489,8 +1633,12 @@
       <c r="H27" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="25" t="str" cm="1">
+        <f t="array" ref="I27">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B27), SEARCH("model=",GetURL(B27))+5+1, (SEARCH("/#",GetURL(B27)))-(SEARCH("model=",GetURL(B27))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -1515,8 +1663,12 @@
       <c r="H28" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="25" t="str" cm="1">
+        <f t="array" ref="I28">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B28), SEARCH("model=",GetURL(B28))+5+1, (SEARCH("/#",GetURL(B28)))-(SEARCH("model=",GetURL(B28))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1541,8 +1693,12 @@
       <c r="H29" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="25" t="str" cm="1">
+        <f t="array" ref="I29">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B29), SEARCH("model=",GetURL(B29))+5+1, (SEARCH("/#",GetURL(B29)))-(SEARCH("model=",GetURL(B29))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -1567,8 +1723,12 @@
       <c r="H30" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I30" s="25" t="str" cm="1">
+        <f t="array" ref="I30">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B30), SEARCH("model=",GetURL(B30))+5+1, (SEARCH("/#",GetURL(B30)))-(SEARCH("model=",GetURL(B30))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1593,8 +1753,12 @@
       <c r="H31" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I31" s="25" t="str" cm="1">
+        <f t="array" ref="I31">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B31), SEARCH("model=",GetURL(B31))+5+1, (SEARCH("/#",GetURL(B31)))-(SEARCH("model=",GetURL(B31))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -1619,8 +1783,12 @@
       <c r="H32" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I32" s="25" t="str" cm="1">
+        <f t="array" ref="I32">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B32), SEARCH("model=",GetURL(B32))+5+1, (SEARCH("/#",GetURL(B32)))-(SEARCH("model=",GetURL(B32))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1645,8 +1813,12 @@
       <c r="H33" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I33" s="25" t="str" cm="1">
+        <f t="array" ref="I33">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B33), SEARCH("model=",GetURL(B33))+5+1, (SEARCH("/#",GetURL(B33)))-(SEARCH("model=",GetURL(B33))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8">
         <v>33</v>
       </c>
@@ -1671,8 +1843,12 @@
       <c r="H34" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I34" s="25" t="str" cm="1">
+        <f t="array" ref="I34">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B34), SEARCH("model=",GetURL(B34))+5+1, (SEARCH("/#",GetURL(B34)))-(SEARCH("model=",GetURL(B34))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>CCCCCCCCCCCCCCN(CC(=O)O[Na])CC(=O)O[Na]</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1697,8 +1873,12 @@
       <c r="H35" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I35" s="25" t="str" cm="1">
+        <f t="array" ref="I35">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B35), SEARCH("model=",GetURL(B35))+5+1, (SEARCH("/#",GetURL(B35)))-(SEARCH("model=",GetURL(B35))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>N.N.[N+](=O)(O)[O-].[N+](=O)(O)[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].O.O.O.O.[Ce+3]</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8">
         <v>35</v>
       </c>
@@ -1723,8 +1903,12 @@
       <c r="H36" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I36" s="25" t="str" cm="1">
+        <f t="array" ref="I36">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B36), SEARCH("model=",GetURL(B36))+5+1, (SEARCH("/#",GetURL(B36)))-(SEARCH("model=",GetURL(B36))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1749,8 +1933,12 @@
       <c r="H37" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I37" s="25" t="str" cm="1">
+        <f t="array" ref="I37">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B37), SEARCH("model=",GetURL(B37))+5+1, (SEARCH("/#",GetURL(B37)))-(SEARCH("model=",GetURL(B37))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8">
         <v>37</v>
       </c>
@@ -1775,8 +1963,12 @@
       <c r="H38" s="10">
         <v>96</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I38" s="25" t="str" cm="1">
+        <f t="array" ref="I38">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B38), SEARCH("model=",GetURL(B38))+5+1, (SEARCH("/#",GetURL(B38)))-(SEARCH("model=",GetURL(B38))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1801,8 +1993,12 @@
       <c r="H39" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I39" s="25" t="str" cm="1">
+        <f t="array" ref="I39">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B39), SEARCH("model=",GetURL(B39))+5+1, (SEARCH("/#",GetURL(B39)))-(SEARCH("model=",GetURL(B39))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8">
         <v>39</v>
       </c>
@@ -1827,8 +2023,12 @@
       <c r="H40" s="10">
         <v>97</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I40" s="25" t="str" cm="1">
+        <f t="array" ref="I40">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B40), SEARCH("model=",GetURL(B40))+5+1, (SEARCH("/#",GetURL(B40)))-(SEARCH("model=",GetURL(B40))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1853,8 +2053,12 @@
       <c r="H41" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I41" s="25" t="str" cm="1">
+        <f t="array" ref="I41">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B41), SEARCH("model=",GetURL(B41))+5+1, (SEARCH("/#",GetURL(B41)))-(SEARCH("model=",GetURL(B41))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8">
         <v>41</v>
       </c>
@@ -1879,8 +2083,12 @@
       <c r="H42" s="10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I42" s="25" t="str" cm="1">
+        <f t="array" ref="I42">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B42), SEARCH("model=",GetURL(B42))+5+1, (SEARCH("/#",GetURL(B42)))-(SEARCH("model=",GetURL(B42))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -1905,8 +2113,12 @@
       <c r="H43" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I43" s="25" t="str" cm="1">
+        <f t="array" ref="I43">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B43), SEARCH("model=",GetURL(B43))+5+1, (SEARCH("/#",GetURL(B43)))-(SEARCH("model=",GetURL(B43))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8">
         <v>43</v>
       </c>
@@ -1931,8 +2143,12 @@
       <c r="H44" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I44" s="25" t="str" cm="1">
+        <f t="array" ref="I44">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B44), SEARCH("model=",GetURL(B44))+5+1, (SEARCH("/#",GetURL(B44)))-(SEARCH("model=",GetURL(B44))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -1957,8 +2173,12 @@
       <c r="H45" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I45" s="25" t="str" cm="1">
+        <f t="array" ref="I45">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B45), SEARCH("model=",GetURL(B45))+5+1, (SEARCH("/#",GetURL(B45)))-(SEARCH("model=",GetURL(B45))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="8">
         <v>45</v>
       </c>
@@ -1983,8 +2203,12 @@
       <c r="H46" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I46" s="25" t="str" cm="1">
+        <f t="array" ref="I46">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B46), SEARCH("model=",GetURL(B46))+5+1, (SEARCH("/#",GetURL(B46)))-(SEARCH("model=",GetURL(B46))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2009,8 +2233,12 @@
       <c r="H47" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I47" s="25" t="str" cm="1">
+        <f t="array" ref="I47">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B47), SEARCH("model=",GetURL(B47))+5+1, (SEARCH("/#",GetURL(B47)))-(SEARCH("model=",GetURL(B47))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="8">
         <v>47</v>
       </c>
@@ -2035,8 +2263,12 @@
       <c r="H48" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I48" s="25" t="str" cm="1">
+        <f t="array" ref="I48">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B48), SEARCH("model=",GetURL(B48))+5+1, (SEARCH("/#",GetURL(B48)))-(SEARCH("model=",GetURL(B48))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -2061,8 +2293,12 @@
       <c r="H49" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I49" s="25" t="str" cm="1">
+        <f t="array" ref="I49">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B49), SEARCH("model=",GetURL(B49))+5+1, (SEARCH("/#",GetURL(B49)))-(SEARCH("model=",GetURL(B49))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -2087,8 +2323,12 @@
       <c r="H50" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I50" s="25" t="str" cm="1">
+        <f t="array" ref="I50">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B50), SEARCH("model=",GetURL(B50))+5+1, (SEARCH("/#",GetURL(B50)))-(SEARCH("model=",GetURL(B50))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -2113,8 +2353,12 @@
       <c r="H51" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I51" s="25" t="str" cm="1">
+        <f t="array" ref="I51">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B51), SEARCH("model=",GetURL(B51))+5+1, (SEARCH("/#",GetURL(B51)))-(SEARCH("model=",GetURL(B51))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="8">
         <v>51</v>
       </c>
@@ -2139,8 +2383,12 @@
       <c r="H52" s="10">
         <v>93</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I52" s="25" t="str" cm="1">
+        <f t="array" ref="I52">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B52), SEARCH("model=",GetURL(B52))+5+1, (SEARCH("/#",GetURL(B52)))-(SEARCH("model=",GetURL(B52))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -2165,8 +2413,12 @@
       <c r="H53" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I53" s="25" t="str" cm="1">
+        <f t="array" ref="I53">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B53), SEARCH("model=",GetURL(B53))+5+1, (SEARCH("/#",GetURL(B53)))-(SEARCH("model=",GetURL(B53))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="8">
         <v>53</v>
       </c>
@@ -2191,8 +2443,12 @@
       <c r="H54" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I54" s="25" t="str" cm="1">
+        <f t="array" ref="I54">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B54), SEARCH("model=",GetURL(B54))+5+1, (SEARCH("/#",GetURL(B54)))-(SEARCH("model=",GetURL(B54))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -2217,8 +2473,12 @@
       <c r="H55" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I55" s="25" t="str" cm="1">
+        <f t="array" ref="I55">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B55), SEARCH("model=",GetURL(B55))+5+1, (SEARCH("/#",GetURL(B55)))-(SEARCH("model=",GetURL(B55))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="8">
         <v>55</v>
       </c>
@@ -2243,8 +2503,12 @@
       <c r="H56" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I56" s="25" t="str" cm="1">
+        <f t="array" ref="I56">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B56), SEARCH("model=",GetURL(B56))+5+1, (SEARCH("/#",GetURL(B56)))-(SEARCH("model=",GetURL(B56))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[Cl-].[Cl-].[Cl-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -2269,8 +2533,12 @@
       <c r="H57" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I57" s="25" t="str" cm="1">
+        <f t="array" ref="I57">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B57), SEARCH("model=",GetURL(B57))+5+1, (SEARCH("/#",GetURL(B57)))-(SEARCH("model=",GetURL(B57))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[Cl-].[Cl-].[Cl-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="8">
         <v>57</v>
       </c>
@@ -2295,8 +2563,12 @@
       <c r="H58" s="10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I58" s="25" t="str" cm="1">
+        <f t="array" ref="I58">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B58), SEARCH("model=",GetURL(B58))+5+1, (SEARCH("/#",GetURL(B58)))-(SEARCH("model=",GetURL(B58))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -2321,8 +2593,12 @@
       <c r="H59" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I59" s="25" t="str" cm="1">
+        <f t="array" ref="I59">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B59), SEARCH("model=",GetURL(B59))+5+1, (SEARCH("/#",GetURL(B59)))-(SEARCH("model=",GetURL(B59))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="8">
         <v>59</v>
       </c>
@@ -2347,8 +2623,12 @@
       <c r="H60" s="10">
         <v>96</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I60" s="25" t="str" cm="1">
+        <f t="array" ref="I60">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B60), SEARCH("model=",GetURL(B60))+5+1, (SEARCH("/#",GetURL(B60)))-(SEARCH("model=",GetURL(B60))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -2373,8 +2653,12 @@
       <c r="H61" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I61" s="25" t="str" cm="1">
+        <f t="array" ref="I61">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B61), SEARCH("model=",GetURL(B61))+5+1, (SEARCH("/#",GetURL(B61)))-(SEARCH("model=",GetURL(B61))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="8">
         <v>61</v>
       </c>
@@ -2399,8 +2683,12 @@
       <c r="H62" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I62" s="25" t="str" cm="1">
+        <f t="array" ref="I62">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B62), SEARCH("model=",GetURL(B62))+5+1, (SEARCH("/#",GetURL(B62)))-(SEARCH("model=",GetURL(B62))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -2425,8 +2713,12 @@
       <c r="H63" s="7">
         <v>91</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I63" s="25" t="str" cm="1">
+        <f t="array" ref="I63">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B63), SEARCH("model=",GetURL(B63))+5+1, (SEARCH("/#",GetURL(B63)))-(SEARCH("model=",GetURL(B63))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="8">
         <v>63</v>
       </c>
@@ -2451,8 +2743,12 @@
       <c r="H64" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I64" s="25" t="str" cm="1">
+        <f t="array" ref="I64">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B64), SEARCH("model=",GetURL(B64))+5+1, (SEARCH("/#",GetURL(B64)))-(SEARCH("model=",GetURL(B64))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -2477,8 +2773,12 @@
       <c r="H65" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I65" s="25" t="str" cm="1">
+        <f t="array" ref="I65">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B65), SEARCH("model=",GetURL(B65))+5+1, (SEARCH("/#",GetURL(B65)))-(SEARCH("model=",GetURL(B65))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="8">
         <v>65</v>
       </c>
@@ -2503,8 +2803,12 @@
       <c r="H66" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I66" s="25" t="str" cm="1">
+        <f t="array" ref="I66">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B66), SEARCH("model=",GetURL(B66))+5+1, (SEARCH("/#",GetURL(B66)))-(SEARCH("model=",GetURL(B66))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -2529,8 +2833,12 @@
       <c r="H67" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I67" s="25" t="str" cm="1">
+        <f t="array" ref="I67">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B67), SEARCH("model=",GetURL(B67))+5+1, (SEARCH("/#",GetURL(B67)))-(SEARCH("model=",GetURL(B67))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[NH4+].[NH4+].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[N+](=O)([O-])[O-].[Ce+4]</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="8">
         <v>67</v>
       </c>
@@ -2555,8 +2863,12 @@
       <c r="H68" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I68" s="25" t="str" cm="1">
+        <f t="array" ref="I68">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B68), SEARCH("model=",GetURL(B68))+5+1, (SEARCH("/#",GetURL(B68)))-(SEARCH("model=",GetURL(B68))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -2581,8 +2893,12 @@
       <c r="H69" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I69" s="25" t="str" cm="1">
+        <f t="array" ref="I69">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B69), SEARCH("model=",GetURL(B69))+5+1, (SEARCH("/#",GetURL(B69)))-(SEARCH("model=",GetURL(B69))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="8">
         <v>69</v>
       </c>
@@ -2607,8 +2923,12 @@
       <c r="H70" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I70" s="25" t="str" cm="1">
+        <f t="array" ref="I70">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B70), SEARCH("model=",GetURL(B70))+5+1, (SEARCH("/#",GetURL(B70)))-(SEARCH("model=",GetURL(B70))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -2633,8 +2953,12 @@
       <c r="H71" s="7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I71" s="25" t="str" cm="1">
+        <f t="array" ref="I71">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B71), SEARCH("model=",GetURL(B71))+5+1, (SEARCH("/#",GetURL(B71)))-(SEARCH("model=",GetURL(B71))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[O-]S(=O)(=O)[O-].[Ce+3].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="8">
         <v>71</v>
       </c>
@@ -2659,8 +2983,12 @@
       <c r="H72" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I72" s="25" t="str" cm="1">
+        <f t="array" ref="I72">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B72), SEARCH("model=",GetURL(B72))+5+1, (SEARCH("/#",GetURL(B72)))-(SEARCH("model=",GetURL(B72))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>[Cl-].[Cl-].[Cl-].[Ce+3]</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -2685,8 +3013,12 @@
       <c r="H73" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I73" s="25" t="str" cm="1">
+        <f t="array" ref="I73">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B73), SEARCH("model=",GetURL(B73))+5+1, (SEARCH("/#",GetURL(B73)))-(SEARCH("model=",GetURL(B73))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>COC1=C(C=CC(=C1)C2=CC(=C(C=C2)N=NC3=C(C4=C(C=C(C=C4C=C3S(=O)(=O)[O-])S(=O)(=O)[O-])N)O)OC)N=NC5=C(C6=C(C=C(C=C6C=C5S(=O)(=O)[O-])S(=O)(=O)[O-])N)O.[Na+].[Na+].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="8">
         <v>73</v>
       </c>
@@ -2711,8 +3043,12 @@
       <c r="H74" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I74" s="25" t="str" cm="1">
+        <f t="array" ref="I74">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B74), SEARCH("model=",GetURL(B74))+5+1, (SEARCH("/#",GetURL(B74)))-(SEARCH("model=",GetURL(B74))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>COC1=C(C=CC(=C1)C2=CC(=C(C=C2)N=NC3=C(C4=C(C=C(C=C4C=C3S(=O)(=O)[O-])S(=O)(=O)[O-])N)O)OC)N=NC5=C(C6=C(C=C(C=C6C=C5S(=O)(=O)[O-])S(=O)(=O)[O-])N)O.[Na+].[Na+].[Na+].[Na+]</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -2737,8 +3073,12 @@
       <c r="H75" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I75" s="25" t="str" cm="1">
+        <f t="array" ref="I75">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B75), SEARCH("model=",GetURL(B75))+5+1, (SEARCH("/#",GetURL(B75)))-(SEARCH("model=",GetURL(B75))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="8">
         <v>75</v>
       </c>
@@ -2763,8 +3103,12 @@
       <c r="H76" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I76" s="25" t="str" cm="1">
+        <f t="array" ref="I76">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B76), SEARCH("model=",GetURL(B76))+5+1, (SEARCH("/#",GetURL(B76)))-(SEARCH("model=",GetURL(B76))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -2789,8 +3133,12 @@
       <c r="H77" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I77" s="25" t="str" cm="1">
+        <f t="array" ref="I77">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B77), SEARCH("model=",GetURL(B77))+5+1, (SEARCH("/#",GetURL(B77)))-(SEARCH("model=",GetURL(B77))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="8">
         <v>77</v>
       </c>
@@ -2815,8 +3163,12 @@
       <c r="H78" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I78" s="25" t="str" cm="1">
+        <f t="array" ref="I78">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B78), SEARCH("model=",GetURL(B78))+5+1, (SEARCH("/#",GetURL(B78)))-(SEARCH("model=",GetURL(B78))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -2841,8 +3193,12 @@
       <c r="H79" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I79" s="25" t="str" cm="1">
+        <f t="array" ref="I79">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B79), SEARCH("model=",GetURL(B79))+5+1, (SEARCH("/#",GetURL(B79)))-(SEARCH("model=",GetURL(B79))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="8">
         <v>79</v>
       </c>
@@ -2867,8 +3223,12 @@
       <c r="H80" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I80" s="25" t="str" cm="1">
+        <f t="array" ref="I80">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B80), SEARCH("model=",GetURL(B80))+5+1, (SEARCH("/#",GetURL(B80)))-(SEARCH("model=",GetURL(B80))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -2893,8 +3253,12 @@
       <c r="H81" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I81" s="25" t="str" cm="1">
+        <f t="array" ref="I81">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B81), SEARCH("model=",GetURL(B81))+5+1, (SEARCH("/#",GetURL(B81)))-(SEARCH("model=",GetURL(B81))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="8">
         <v>81</v>
       </c>
@@ -2919,8 +3283,12 @@
       <c r="H82" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I82" s="25" t="str" cm="1">
+        <f t="array" ref="I82">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B82), SEARCH("model=",GetURL(B82))+5+1, (SEARCH("/#",GetURL(B82)))-(SEARCH("model=",GetURL(B82))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -2945,8 +3313,12 @@
       <c r="H83" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I83" s="25" t="str" cm="1">
+        <f t="array" ref="I83">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B83), SEARCH("model=",GetURL(B83))+5+1, (SEARCH("/#",GetURL(B83)))-(SEARCH("model=",GetURL(B83))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="8">
         <v>83</v>
       </c>
@@ -2971,8 +3343,12 @@
       <c r="H84" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I84" s="25" t="str" cm="1">
+        <f t="array" ref="I84">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B84), SEARCH("model=",GetURL(B84))+5+1, (SEARCH("/#",GetURL(B84)))-(SEARCH("model=",GetURL(B84))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -2997,8 +3373,12 @@
       <c r="H85" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I85" s="25" t="str" cm="1">
+        <f t="array" ref="I85">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B85), SEARCH("model=",GetURL(B85))+5+1, (SEARCH("/#",GetURL(B85)))-(SEARCH("model=",GetURL(B85))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="8">
         <v>85</v>
       </c>
@@ -3023,8 +3403,12 @@
       <c r="H86" s="10">
         <v>90</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I86" s="25" t="str" cm="1">
+        <f t="array" ref="I86">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B86), SEARCH("model=",GetURL(B86))+5+1, (SEARCH("/#",GetURL(B86)))-(SEARCH("model=",GetURL(B86))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -3049,8 +3433,12 @@
       <c r="H87" s="7">
         <v>90</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I87" s="25" t="str" cm="1">
+        <f t="array" ref="I87">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B87), SEARCH("model=",GetURL(B87))+5+1, (SEARCH("/#",GetURL(B87)))-(SEARCH("model=",GetURL(B87))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="8">
         <v>87</v>
       </c>
@@ -3075,8 +3463,12 @@
       <c r="H88" s="10">
         <v>92</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I88" s="25" t="str" cm="1">
+        <f t="array" ref="I88">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B88), SEARCH("model=",GetURL(B88))+5+1, (SEARCH("/#",GetURL(B88)))-(SEARCH("model=",GetURL(B88))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Fe+2]</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -3101,8 +3493,12 @@
       <c r="H89" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I89" s="25" t="str" cm="1">
+        <f t="array" ref="I89">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B89), SEARCH("model=",GetURL(B89))+5+1, (SEARCH("/#",GetURL(B89)))-(SEARCH("model=",GetURL(B89))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="8">
         <v>89</v>
       </c>
@@ -3127,8 +3523,12 @@
       <c r="H90" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I90" s="25" t="str" cm="1">
+        <f t="array" ref="I90">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B90), SEARCH("model=",GetURL(B90))+5+1, (SEARCH("/#",GetURL(B90)))-(SEARCH("model=",GetURL(B90))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -3153,8 +3553,12 @@
       <c r="H91" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I91" s="25" t="str" cm="1">
+        <f t="array" ref="I91">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B91), SEARCH("model=",GetURL(B91))+5+1, (SEARCH("/#",GetURL(B91)))-(SEARCH("model=",GetURL(B91))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="8">
         <v>91</v>
       </c>
@@ -3179,8 +3583,12 @@
       <c r="H92" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I92" s="25" t="str" cm="1">
+        <f t="array" ref="I92">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B92), SEARCH("model=",GetURL(B92))+5+1, (SEARCH("/#",GetURL(B92)))-(SEARCH("model=",GetURL(B92))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -3205,8 +3613,12 @@
       <c r="H93" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I93" s="25" t="str" cm="1">
+        <f t="array" ref="I93">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B93), SEARCH("model=",GetURL(B93))+5+1, (SEARCH("/#",GetURL(B93)))-(SEARCH("model=",GetURL(B93))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="8">
         <v>93</v>
       </c>
@@ -3231,8 +3643,12 @@
       <c r="H94" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I94" s="25" t="str" cm="1">
+        <f t="array" ref="I94">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B94), SEARCH("model=",GetURL(B94))+5+1, (SEARCH("/#",GetURL(B94)))-(SEARCH("model=",GetURL(B94))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -3257,8 +3673,12 @@
       <c r="H95" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I95" s="25" t="str" cm="1">
+        <f t="array" ref="I95">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B95), SEARCH("model=",GetURL(B95))+5+1, (SEARCH("/#",GetURL(B95)))-(SEARCH("model=",GetURL(B95))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="8">
         <v>95</v>
       </c>
@@ -3283,8 +3703,12 @@
       <c r="H96" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I96" s="25" t="str" cm="1">
+        <f t="array" ref="I96">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B96), SEARCH("model=",GetURL(B96))+5+1, (SEARCH("/#",GetURL(B96)))-(SEARCH("model=",GetURL(B96))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -3309,8 +3733,12 @@
       <c r="H97" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I97" s="25" t="str" cm="1">
+        <f t="array" ref="I97">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B97), SEARCH("model=",GetURL(B97))+5+1, (SEARCH("/#",GetURL(B97)))-(SEARCH("model=",GetURL(B97))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8">
         <v>97</v>
       </c>
@@ -3335,8 +3763,12 @@
       <c r="H98" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I98" s="25" t="str" cm="1">
+        <f t="array" ref="I98">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B98), SEARCH("model=",GetURL(B98))+5+1, (SEARCH("/#",GetURL(B98)))-(SEARCH("model=",GetURL(B98))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -3361,8 +3793,12 @@
       <c r="H99" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I99" s="25" t="str" cm="1">
+        <f t="array" ref="I99">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B99), SEARCH("model=",GetURL(B99))+5+1, (SEARCH("/#",GetURL(B99)))-(SEARCH("model=",GetURL(B99))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="12">
         <v>99</v>
       </c>
@@ -3387,8 +3823,12 @@
       <c r="H100" s="14" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I100" s="25" t="str" cm="1">
+        <f t="array" ref="I100">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B100), SEARCH("model=",GetURL(B100))+5+1, (SEARCH("/#",GetURL(B100)))-(SEARCH("model=",GetURL(B100))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="15">
         <v>100</v>
       </c>
@@ -3413,8 +3853,12 @@
       <c r="H101" s="17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I101" s="25" t="str" cm="1">
+        <f t="array" ref="I101">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B101), SEARCH("model=",GetURL(B101))+5+1, (SEARCH("/#",GetURL(B101)))-(SEARCH("model=",GetURL(B101))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -3439,8 +3883,12 @@
       <c r="H102" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I102" s="25" t="str" cm="1">
+        <f t="array" ref="I102">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B102), SEARCH("model=",GetURL(B102))+5+1, (SEARCH("/#",GetURL(B102)))-(SEARCH("model=",GetURL(B102))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -3465,8 +3913,12 @@
       <c r="H103" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I103" s="25" t="str" cm="1">
+        <f t="array" ref="I103">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B103), SEARCH("model=",GetURL(B103))+5+1, (SEARCH("/#",GetURL(B103)))-(SEARCH("model=",GetURL(B103))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="8">
         <v>103</v>
       </c>
@@ -3491,8 +3943,12 @@
       <c r="H104" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I104" s="25" t="str" cm="1">
+        <f t="array" ref="I104">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B104), SEARCH("model=",GetURL(B104))+5+1, (SEARCH("/#",GetURL(B104)))-(SEARCH("model=",GetURL(B104))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -3517,8 +3973,12 @@
       <c r="H105" s="7">
         <v>90</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I105" s="25" t="str" cm="1">
+        <f t="array" ref="I105">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B105), SEARCH("model=",GetURL(B105))+5+1, (SEARCH("/#",GetURL(B105)))-(SEARCH("model=",GetURL(B105))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="8">
         <v>105</v>
       </c>
@@ -3543,8 +4003,12 @@
       <c r="H106" s="10">
         <v>91</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I106" s="25" t="str" cm="1">
+        <f t="array" ref="I106">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B106), SEARCH("model=",GetURL(B106))+5+1, (SEARCH("/#",GetURL(B106)))-(SEARCH("model=",GetURL(B106))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -3569,8 +4033,12 @@
       <c r="H107" s="7">
         <v>91</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I107" s="25" t="str" cm="1">
+        <f t="array" ref="I107">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B107), SEARCH("model=",GetURL(B107))+5+1, (SEARCH("/#",GetURL(B107)))-(SEARCH("model=",GetURL(B107))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="8">
         <v>107</v>
       </c>
@@ -3595,8 +4063,12 @@
       <c r="H108" s="10">
         <v>92</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I108" s="25" t="str" cm="1">
+        <f t="array" ref="I108">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B108), SEARCH("model=",GetURL(B108))+5+1, (SEARCH("/#",GetURL(B108)))-(SEARCH("model=",GetURL(B108))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -3621,8 +4093,12 @@
       <c r="H109" s="7">
         <v>93</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I109" s="25" t="str" cm="1">
+        <f t="array" ref="I109">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B109), SEARCH("model=",GetURL(B109))+5+1, (SEARCH("/#",GetURL(B109)))-(SEARCH("model=",GetURL(B109))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="8">
         <v>109</v>
       </c>
@@ -3647,8 +4123,12 @@
       <c r="H110" s="10">
         <v>94</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I110" s="25" t="str" cm="1">
+        <f t="array" ref="I110">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B110), SEARCH("model=",GetURL(B110))+5+1, (SEARCH("/#",GetURL(B110)))-(SEARCH("model=",GetURL(B110))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C(C(C(C(C(C(=O)[O-])O)O)O)O)O.C(C(C(C(C(C(=O)[O-])O)O)O)O)O.[Zn+2]</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -3673,8 +4153,12 @@
       <c r="H111" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I111" s="25" t="str" cm="1">
+        <f t="array" ref="I111">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B111), SEARCH("model=",GetURL(B111))+5+1, (SEARCH("/#",GetURL(B111)))-(SEARCH("model=",GetURL(B111))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC(=C(C=C1O)O)C=NNC(=S)N</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="8">
         <v>111</v>
       </c>
@@ -3699,8 +4183,12 @@
       <c r="H112" s="10">
         <v>90</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I112" s="25" t="str" cm="1">
+        <f t="array" ref="I112">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B112), SEARCH("model=",GetURL(B112))+5+1, (SEARCH("/#",GetURL(B112)))-(SEARCH("model=",GetURL(B112))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC(=C(C=C1O)O)C=NNC(=S)N</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -3725,8 +4213,12 @@
       <c r="H113" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I113" s="25" t="str" cm="1">
+        <f t="array" ref="I113">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B113), SEARCH("model=",GetURL(B113))+5+1, (SEARCH("/#",GetURL(B113)))-(SEARCH("model=",GetURL(B113))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>NC(=S)NN=CC1=C(C(=C(C=C1)O)O)O</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="8">
         <v>113</v>
       </c>
@@ -3751,8 +4243,12 @@
       <c r="H114" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I114" s="25" t="str" cm="1">
+        <f t="array" ref="I114">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B114), SEARCH("model=",GetURL(B114))+5+1, (SEARCH("/#",GetURL(B114)))-(SEARCH("model=",GetURL(B114))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>NC(=S)NN=CC1=C(C(=C(C=C1)O)O)O</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -3777,8 +4273,12 @@
       <c r="H115" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I115" s="25" t="str" cm="1">
+        <f t="array" ref="I115">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B115), SEARCH("model=",GetURL(B115))+5+1, (SEARCH("/#",GetURL(B115)))-(SEARCH("model=",GetURL(B115))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>NC(=S)NN=CC1=C(C(=C(C=C1)O)O)O</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="8">
         <v>115</v>
       </c>
@@ -3803,8 +4303,12 @@
       <c r="H116" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I116" s="25" t="str" cm="1">
+        <f t="array" ref="I116">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B116), SEARCH("model=",GetURL(B116))+5+1, (SEARCH("/#",GetURL(B116)))-(SEARCH("model=",GetURL(B116))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>NC(=S)NN=CC1=C(C(=C(C=C1)O)O)O</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -3829,8 +4333,12 @@
       <c r="H117" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I117" s="25" t="str" cm="1">
+        <f t="array" ref="I117">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B117), SEARCH("model=",GetURL(B117))+5+1, (SEARCH("/#",GetURL(B117)))-(SEARCH("model=",GetURL(B117))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>NC(=S)NN=CC1=C(C(=C(C=C1)O)O)O</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="8">
         <v>117</v>
       </c>
@@ -3855,8 +4363,12 @@
       <c r="H118" s="10">
         <v>94</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I118" s="25" t="str" cm="1">
+        <f t="array" ref="I118">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B118), SEARCH("model=",GetURL(B118))+5+1, (SEARCH("/#",GetURL(B118)))-(SEARCH("model=",GetURL(B118))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C=CCN(CC=C)C1=NC(=NC(=N1)S)S[Na]</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>118</v>
       </c>
@@ -3881,8 +4393,12 @@
       <c r="H119" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I119" s="25" t="str" cm="1">
+        <f t="array" ref="I119">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B119), SEARCH("model=",GetURL(B119))+5+1, (SEARCH("/#",GetURL(B119)))-(SEARCH("model=",GetURL(B119))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>c1ccc2c(c1)[nH]nn2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="8">
         <v>119</v>
       </c>
@@ -3907,8 +4423,12 @@
       <c r="H120" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I120" s="25" t="str" cm="1">
+        <f t="array" ref="I120">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B120), SEARCH("model=",GetURL(B120))+5+1, (SEARCH("/#",GetURL(B120)))-(SEARCH("model=",GetURL(B120))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>c1ccc2c(c1)[nH]nn2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -3933,8 +4453,12 @@
       <c r="H121" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I121" s="25" t="str" cm="1">
+        <f t="array" ref="I121">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B121), SEARCH("model=",GetURL(B121))+5+1, (SEARCH("/#",GetURL(B121)))-(SEARCH("model=",GetURL(B121))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC2=NNN=C2C=C1Cl</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="8">
         <v>121</v>
       </c>
@@ -3959,8 +4483,12 @@
       <c r="H122" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I122" s="25" t="str" cm="1">
+        <f t="array" ref="I122">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B122), SEARCH("model=",GetURL(B122))+5+1, (SEARCH("/#",GetURL(B122)))-(SEARCH("model=",GetURL(B122))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>C1=CC2=NNN=C2C=C1Cl</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -3985,8 +4513,12 @@
       <c r="H123" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I123" s="25" t="str" cm="1">
+        <f t="array" ref="I123">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B123), SEARCH("model=",GetURL(B123))+5+1, (SEARCH("/#",GetURL(B123)))-(SEARCH("model=",GetURL(B123))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>COC(=O)n1nnc2ccccc12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="12">
         <v>123</v>
       </c>
@@ -4011,8 +4543,12 @@
       <c r="H124" s="14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I124" s="25" t="str" cm="1">
+        <f t="array" ref="I124">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B124), SEARCH("model=",GetURL(B124))+5+1, (SEARCH("/#",GetURL(B124)))-(SEARCH("model=",GetURL(B124))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>COC(=O)n1nnc2ccccc12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>124</v>
       </c>
@@ -4037,8 +4573,12 @@
       <c r="H125" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I125" s="25" t="str" cm="1">
+        <f t="array" ref="I125">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B125), SEARCH("model=",GetURL(B125))+5+1, (SEARCH("/#",GetURL(B125)))-(SEARCH("model=",GetURL(B125))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>S=c1sc2c([nH]1)cccc2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="18">
         <v>125</v>
       </c>
@@ -4062,6 +4602,10 @@
       </c>
       <c r="H126" s="20" t="s">
         <v>99</v>
+      </c>
+      <c r="I126" s="25" t="str" cm="1">
+        <f t="array" ref="I126">SUBSTITUTE(SUBSTITUTE(MIDB(GetURL(B126), SEARCH("model=",GetURL(B126))+5+1, (SEARCH("/#",GetURL(B126)))-(SEARCH("model=",GetURL(B126))+5+1)), "%5b", "["), "%5d", "]")</f>
+        <v>S=c1sc2c([nH]1)cccc2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>